<commit_message>
Added library and updated BOM.
</commit_message>
<xml_diff>
--- a/PCB modules/servo driver/harp expander servo driver v1.0 BOM.xlsx
+++ b/PCB modules/servo driver/harp expander servo driver v1.0 BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_expander\PCB modules\servo driver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Google Drive\projects\harp-tech\harp_expander\PCB modules - servo driver v1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5216E8EF-458D-44E1-8588-5892776018FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE269C6-6072-4CD1-92A4-B17835B6A21E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22DE42AE-D7DB-44FC-B9CF-DE1961A005DB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22DE42AE-D7DB-44FC-B9CF-DE1961A005DB}"/>
   </bookViews>
   <sheets>
     <sheet name="harp expander v1" sheetId="1" r:id="rId1"/>
@@ -192,6 +192,9 @@
     <t>100nF</t>
   </si>
   <si>
+    <t>445-6899-2-ND</t>
+  </si>
+  <si>
     <t>CGA2B3X7R1H104K050BB</t>
   </si>
   <si>
@@ -393,13 +396,10 @@
     <t>Mouser</t>
   </si>
   <si>
+    <t>SI8641AB-B-IS</t>
+  </si>
+  <si>
     <t>SI8641AB-B-IS-ND</t>
-  </si>
-  <si>
-    <t>SI8641AB-B-IS</t>
-  </si>
-  <si>
-    <t>445-6899-1-ND</t>
   </si>
 </sst>
 </file>
@@ -1335,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34:F37"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,7 +1399,7 @@
         <v>113</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>36</v>
@@ -1411,10 +1411,10 @@
         <v>10</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1422,25 +1422,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>37</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1448,25 +1448,25 @@
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>38</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1483,16 +1483,16 @@
         <v>22</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>114</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1500,7 +1500,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>5</v>
@@ -1509,16 +1509,16 @@
         <v>27</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1526,7 +1526,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>5</v>
@@ -1535,16 +1535,16 @@
         <v>28</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1552,7 +1552,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>5</v>
@@ -1561,16 +1561,16 @@
         <v>24</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1578,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>23</v>
@@ -1587,16 +1587,16 @@
         <v>25</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1604,7 +1604,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>5</v>
@@ -1613,16 +1613,16 @@
         <v>26</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1630,7 +1630,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>30</v>
@@ -1639,16 +1639,16 @@
         <v>29</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1656,25 +1656,25 @@
         <v>2</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F13" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1682,25 +1682,25 @@
         <v>1</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F14" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1708,25 +1708,25 @@
         <v>1</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>32</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1734,25 +1734,25 @@
         <v>1</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>33</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F16" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1760,25 +1760,25 @@
         <v>1</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>40</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F17" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1786,25 +1786,25 @@
         <v>1</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>39</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F18" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1812,25 +1812,25 @@
         <v>3</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F19" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1838,25 +1838,25 @@
         <v>1</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1867,7 +1867,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>35</v>
@@ -1879,7 +1879,7 @@
         <v>11</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>43</v>
@@ -1907,25 +1907,25 @@
         <v>20</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
@@ -1938,25 +1938,25 @@
         <v>14</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
@@ -1969,25 +1969,25 @@
         <v>15</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -2028,6 +2028,30 @@
       </c>
       <c r="F29" s="1">
         <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="1">
+        <f>12/5</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="1">
+        <f>3/F34</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="1">
+        <f>1.5/F35</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="1">
+        <f>1.25/1.5</f>
+        <v>0.83333333333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>